<commit_message>
Try to fix save of new item.
</commit_message>
<xml_diff>
--- a/karelsluka.xlsx
+++ b/karelsluka.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="21">
   <si>
     <t xml:space="preserve">datum</t>
   </si>
@@ -326,15 +326,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BL104"/>
+  <dimension ref="A1:BL114"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="5.1"/>
@@ -386,7 +386,7 @@
     </row>
     <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="n">
-        <v>44518</v>
+        <v>44528</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>1</v>
@@ -427,7 +427,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="n">
-        <v>44517</v>
+        <v>44527</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>1</v>
@@ -442,7 +442,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" s="7" t="n">
         <v>1</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="n">
-        <v>44516</v>
+        <v>44526</v>
       </c>
       <c r="B4" s="7" t="n">
         <v>1</v>
@@ -509,13 +509,13 @@
     </row>
     <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="n">
-        <v>44515</v>
+        <v>44525</v>
       </c>
       <c r="B5" s="7" t="n">
         <v>1</v>
       </c>
       <c r="C5" s="7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="7" t="n">
         <v>1</v>
@@ -550,7 +550,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="n">
-        <v>44514</v>
+        <v>44524</v>
       </c>
       <c r="B6" s="7" t="n">
         <v>1</v>
@@ -559,7 +559,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" s="7" t="n">
         <v>1</v>
@@ -571,7 +571,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I6" s="7" t="n">
         <v>1</v>
@@ -586,12 +586,12 @@
         <v>1</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="n">
-        <v>44513</v>
+        <v>44523</v>
       </c>
       <c r="B7" s="7" t="n">
         <v>1</v>
@@ -624,15 +624,15 @@
         <v>1</v>
       </c>
       <c r="L7" s="7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="n">
-        <v>44511</v>
+        <v>44522</v>
       </c>
       <c r="B8" s="7" t="n">
         <v>1</v>
@@ -673,7 +673,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="n">
-        <v>44510</v>
+        <v>44521</v>
       </c>
       <c r="B9" s="7" t="n">
         <v>1</v>
@@ -682,13 +682,13 @@
         <v>1</v>
       </c>
       <c r="D9" s="7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" s="7" t="n">
         <v>1</v>
       </c>
       <c r="F9" s="7" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G9" s="7" t="n">
         <v>1</v>
@@ -709,12 +709,12 @@
         <v>1</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="n">
-        <v>44509</v>
+        <v>44520</v>
       </c>
       <c r="B10" s="7" t="n">
         <v>1</v>
@@ -723,13 +723,13 @@
         <v>1</v>
       </c>
       <c r="D10" s="7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10" s="7" t="n">
         <v>1</v>
       </c>
       <c r="F10" s="7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G10" s="7" t="n">
         <v>1</v>
@@ -750,12 +750,12 @@
         <v>1</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="n">
-        <v>44508</v>
+        <v>44519</v>
       </c>
       <c r="B11" s="7" t="n">
         <v>1</v>
@@ -764,13 +764,13 @@
         <v>1</v>
       </c>
       <c r="D11" s="7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11" s="7" t="n">
         <v>1</v>
       </c>
       <c r="F11" s="7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11" s="7" t="n">
         <v>1</v>
@@ -796,7 +796,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="n">
-        <v>44507</v>
+        <v>44518</v>
       </c>
       <c r="B12" s="7" t="n">
         <v>1</v>
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G12" s="7" t="n">
         <v>1</v>
@@ -832,12 +832,12 @@
         <v>1</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="n">
-        <v>44506</v>
+        <v>44517</v>
       </c>
       <c r="B13" s="7" t="n">
         <v>1</v>
@@ -873,12 +873,12 @@
         <v>1</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="n">
-        <v>44505</v>
+        <v>44516</v>
       </c>
       <c r="B14" s="7" t="n">
         <v>1</v>
@@ -919,13 +919,13 @@
     </row>
     <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="n">
-        <v>44504</v>
+        <v>44515</v>
       </c>
       <c r="B15" s="7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" s="7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="7" t="n">
         <v>1</v>
@@ -934,7 +934,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="7" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G15" s="7" t="n">
         <v>1</v>
@@ -960,7 +960,7 @@
     </row>
     <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="n">
-        <v>44503</v>
+        <v>44514</v>
       </c>
       <c r="B16" s="7" t="n">
         <v>1</v>
@@ -975,13 +975,13 @@
         <v>1</v>
       </c>
       <c r="F16" s="7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G16" s="7" t="n">
         <v>1</v>
       </c>
       <c r="H16" s="7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I16" s="7" t="n">
         <v>1</v>
@@ -996,12 +996,12 @@
         <v>1</v>
       </c>
       <c r="M16" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="n">
-        <v>44502</v>
+        <v>44513</v>
       </c>
       <c r="B17" s="7" t="n">
         <v>1</v>
@@ -1022,7 +1022,7 @@
         <v>1</v>
       </c>
       <c r="H17" s="7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I17" s="7" t="n">
         <v>1</v>
@@ -1034,15 +1034,15 @@
         <v>1</v>
       </c>
       <c r="L17" s="7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="n">
-        <v>44501</v>
+        <v>44511</v>
       </c>
       <c r="B18" s="7" t="n">
         <v>1</v>
@@ -1083,7 +1083,7 @@
     </row>
     <row r="19" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="n">
-        <v>44500</v>
+        <v>44510</v>
       </c>
       <c r="B19" s="7" t="n">
         <v>1</v>
@@ -1092,13 +1092,13 @@
         <v>1</v>
       </c>
       <c r="D19" s="7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19" s="7" t="n">
         <v>1</v>
       </c>
       <c r="F19" s="7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G19" s="7" t="n">
         <v>1</v>
@@ -1118,11 +1118,13 @@
       <c r="L19" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="M19" s="7"/>
+      <c r="M19" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="n">
-        <v>44499</v>
+        <v>44509</v>
       </c>
       <c r="B20" s="7" t="n">
         <v>1</v>
@@ -1131,7 +1133,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20" s="7" t="n">
         <v>1</v>
@@ -1157,11 +1159,13 @@
       <c r="L20" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="M20" s="7"/>
+      <c r="M20" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="n">
-        <v>44498</v>
+        <v>44508</v>
       </c>
       <c r="B21" s="7" t="n">
         <v>1</v>
@@ -1170,13 +1174,13 @@
         <v>1</v>
       </c>
       <c r="D21" s="7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21" s="7" t="n">
         <v>1</v>
       </c>
       <c r="F21" s="7" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G21" s="7" t="n">
         <v>1</v>
@@ -1196,11 +1200,13 @@
       <c r="L21" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="M21" s="7"/>
+      <c r="M21" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="n">
-        <v>44497</v>
+        <v>44507</v>
       </c>
       <c r="B22" s="7" t="n">
         <v>1</v>
@@ -1235,11 +1241,13 @@
       <c r="L22" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="M22" s="7"/>
+      <c r="M22" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="n">
-        <v>44496</v>
+        <v>44506</v>
       </c>
       <c r="B23" s="7" t="n">
         <v>1</v>
@@ -1275,12 +1283,12 @@
         <v>1</v>
       </c>
       <c r="M23" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="n">
-        <v>44495</v>
+        <v>44505</v>
       </c>
       <c r="B24" s="7" t="n">
         <v>1</v>
@@ -1315,14 +1323,16 @@
       <c r="L24" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="M24" s="7"/>
+      <c r="M24" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="n">
-        <v>44494</v>
+        <v>44504</v>
       </c>
       <c r="B25" s="7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25" s="7" t="n">
         <v>1</v>
@@ -1334,7 +1344,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="7" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G25" s="7" t="n">
         <v>1</v>
@@ -1354,11 +1364,13 @@
       <c r="L25" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="M25" s="7"/>
+      <c r="M25" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="n">
-        <v>44493</v>
+        <v>44503</v>
       </c>
       <c r="B26" s="7" t="n">
         <v>1</v>
@@ -1373,7 +1385,7 @@
         <v>1</v>
       </c>
       <c r="F26" s="7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G26" s="7" t="n">
         <v>1</v>
@@ -1393,11 +1405,13 @@
       <c r="L26" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="M26" s="7"/>
+      <c r="M26" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="n">
-        <v>44492</v>
+        <v>44502</v>
       </c>
       <c r="B27" s="7" t="n">
         <v>1</v>
@@ -1412,13 +1426,13 @@
         <v>1</v>
       </c>
       <c r="F27" s="7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G27" s="7" t="n">
         <v>1</v>
       </c>
       <c r="H27" s="7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I27" s="7" t="n">
         <v>1</v>
@@ -1432,11 +1446,13 @@
       <c r="L27" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="M27" s="7"/>
+      <c r="M27" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="n">
-        <v>44490</v>
+        <v>44501</v>
       </c>
       <c r="B28" s="7" t="n">
         <v>1</v>
@@ -1471,11 +1487,13 @@
       <c r="L28" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="M28" s="7"/>
+      <c r="M28" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="n">
-        <v>44489</v>
+        <v>44500</v>
       </c>
       <c r="B29" s="7" t="n">
         <v>1</v>
@@ -1490,7 +1508,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="7" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G29" s="7" t="n">
         <v>1</v>
@@ -1514,7 +1532,7 @@
     </row>
     <row r="30" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="n">
-        <v>44488</v>
+        <v>44499</v>
       </c>
       <c r="B30" s="7" t="n">
         <v>1</v>
@@ -1523,13 +1541,13 @@
         <v>1</v>
       </c>
       <c r="D30" s="7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E30" s="7" t="n">
         <v>1</v>
       </c>
       <c r="F30" s="7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G30" s="7" t="n">
         <v>1</v>
@@ -1553,7 +1571,7 @@
     </row>
     <row r="31" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="n">
-        <v>44487</v>
+        <v>44498</v>
       </c>
       <c r="B31" s="7" t="n">
         <v>1</v>
@@ -1568,7 +1586,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="7" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G31" s="7" t="n">
         <v>1</v>
@@ -1592,7 +1610,7 @@
     </row>
     <row r="32" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="n">
-        <v>44486</v>
+        <v>44497</v>
       </c>
       <c r="B32" s="7" t="n">
         <v>1</v>
@@ -1601,13 +1619,13 @@
         <v>1</v>
       </c>
       <c r="D32" s="7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E32" s="7" t="n">
         <v>1</v>
       </c>
       <c r="F32" s="7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G32" s="7" t="n">
         <v>1</v>
@@ -1631,7 +1649,7 @@
     </row>
     <row r="33" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="n">
-        <v>44485</v>
+        <v>44496</v>
       </c>
       <c r="B33" s="7" t="n">
         <v>1</v>
@@ -1652,7 +1670,7 @@
         <v>1</v>
       </c>
       <c r="H33" s="7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I33" s="7" t="n">
         <v>1</v>
@@ -1666,11 +1684,13 @@
       <c r="L33" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="M33" s="7"/>
+      <c r="M33" s="7" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="n">
-        <v>44484</v>
+        <v>44495</v>
       </c>
       <c r="B34" s="7" t="n">
         <v>1</v>
@@ -1709,7 +1729,7 @@
     </row>
     <row r="35" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="n">
-        <v>44483</v>
+        <v>44494</v>
       </c>
       <c r="B35" s="7" t="n">
         <v>1</v>
@@ -1724,7 +1744,7 @@
         <v>1</v>
       </c>
       <c r="F35" s="7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G35" s="7" t="n">
         <v>1</v>
@@ -1748,7 +1768,7 @@
     </row>
     <row r="36" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="n">
-        <v>44482</v>
+        <v>44493</v>
       </c>
       <c r="B36" s="7" t="n">
         <v>1</v>
@@ -1763,7 +1783,7 @@
         <v>1</v>
       </c>
       <c r="F36" s="7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G36" s="7" t="n">
         <v>1</v>
@@ -1787,7 +1807,7 @@
     </row>
     <row r="37" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="n">
-        <v>44481</v>
+        <v>44492</v>
       </c>
       <c r="B37" s="7" t="n">
         <v>1</v>
@@ -1802,7 +1822,7 @@
         <v>1</v>
       </c>
       <c r="F37" s="7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G37" s="7" t="n">
         <v>1</v>
@@ -1826,7 +1846,7 @@
     </row>
     <row r="38" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="n">
-        <v>44480</v>
+        <v>44490</v>
       </c>
       <c r="B38" s="7" t="n">
         <v>1</v>
@@ -1835,13 +1855,13 @@
         <v>1</v>
       </c>
       <c r="D38" s="7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E38" s="7" t="n">
         <v>1</v>
       </c>
       <c r="F38" s="7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G38" s="7" t="n">
         <v>1</v>
@@ -1865,7 +1885,7 @@
     </row>
     <row r="39" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="6" t="n">
-        <v>44479</v>
+        <v>44489</v>
       </c>
       <c r="B39" s="7" t="n">
         <v>1</v>
@@ -1880,7 +1900,7 @@
         <v>1</v>
       </c>
       <c r="F39" s="7" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G39" s="7" t="n">
         <v>1</v>
@@ -1904,7 +1924,7 @@
     </row>
     <row r="40" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="6" t="n">
-        <v>44477</v>
+        <v>44488</v>
       </c>
       <c r="B40" s="7" t="n">
         <v>1</v>
@@ -1913,13 +1933,13 @@
         <v>1</v>
       </c>
       <c r="D40" s="7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E40" s="7" t="n">
         <v>1</v>
       </c>
       <c r="F40" s="7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G40" s="7" t="n">
         <v>1</v>
@@ -1943,7 +1963,7 @@
     </row>
     <row r="41" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="n">
-        <v>44476</v>
+        <v>44487</v>
       </c>
       <c r="B41" s="7" t="n">
         <v>1</v>
@@ -1952,7 +1972,7 @@
         <v>1</v>
       </c>
       <c r="D41" s="7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E41" s="7" t="n">
         <v>1</v>
@@ -1982,7 +2002,7 @@
     </row>
     <row r="42" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="6" t="n">
-        <v>44475</v>
+        <v>44486</v>
       </c>
       <c r="B42" s="7" t="n">
         <v>1</v>
@@ -1991,7 +2011,7 @@
         <v>1</v>
       </c>
       <c r="D42" s="7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E42" s="7" t="n">
         <v>1</v>
@@ -2021,7 +2041,7 @@
     </row>
     <row r="43" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="6" t="n">
-        <v>44474</v>
+        <v>44485</v>
       </c>
       <c r="B43" s="7" t="n">
         <v>1</v>
@@ -2042,7 +2062,7 @@
         <v>1</v>
       </c>
       <c r="H43" s="7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I43" s="7" t="n">
         <v>1</v>
@@ -2060,7 +2080,7 @@
     </row>
     <row r="44" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="n">
-        <v>44473</v>
+        <v>44484</v>
       </c>
       <c r="B44" s="7" t="n">
         <v>1</v>
@@ -2099,7 +2119,7 @@
     </row>
     <row r="45" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="n">
-        <v>44472</v>
+        <v>44483</v>
       </c>
       <c r="B45" s="7" t="n">
         <v>1</v>
@@ -2138,10 +2158,10 @@
     </row>
     <row r="46" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="n">
-        <v>44471</v>
+        <v>44482</v>
       </c>
       <c r="B46" s="7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C46" s="7" t="n">
         <v>1</v>
@@ -2177,7 +2197,7 @@
     </row>
     <row r="47" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="n">
-        <v>44470</v>
+        <v>44481</v>
       </c>
       <c r="B47" s="7" t="n">
         <v>1</v>
@@ -2216,7 +2236,7 @@
     </row>
     <row r="48" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="n">
-        <v>44469</v>
+        <v>44480</v>
       </c>
       <c r="B48" s="7" t="n">
         <v>1</v>
@@ -2225,13 +2245,13 @@
         <v>1</v>
       </c>
       <c r="D48" s="7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E48" s="7" t="n">
         <v>1</v>
       </c>
       <c r="F48" s="7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G48" s="7" t="n">
         <v>1</v>
@@ -2255,7 +2275,7 @@
     </row>
     <row r="49" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="6" t="n">
-        <v>44468</v>
+        <v>44479</v>
       </c>
       <c r="B49" s="7" t="n">
         <v>1</v>
@@ -2270,7 +2290,7 @@
         <v>1</v>
       </c>
       <c r="F49" s="7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G49" s="7" t="n">
         <v>1</v>
@@ -2294,7 +2314,7 @@
     </row>
     <row r="50" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="6" t="n">
-        <v>44467</v>
+        <v>44477</v>
       </c>
       <c r="B50" s="7" t="n">
         <v>1</v>
@@ -2309,7 +2329,7 @@
         <v>1</v>
       </c>
       <c r="F50" s="7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G50" s="7" t="n">
         <v>1</v>
@@ -2333,7 +2353,7 @@
     </row>
     <row r="51" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="6" t="n">
-        <v>44466</v>
+        <v>44476</v>
       </c>
       <c r="B51" s="7" t="n">
         <v>1</v>
@@ -2342,7 +2362,7 @@
         <v>1</v>
       </c>
       <c r="D51" s="7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E51" s="7" t="n">
         <v>1</v>
@@ -2372,7 +2392,7 @@
     </row>
     <row r="52" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="6" t="n">
-        <v>44465</v>
+        <v>44475</v>
       </c>
       <c r="B52" s="7" t="n">
         <v>1</v>
@@ -2381,7 +2401,7 @@
         <v>1</v>
       </c>
       <c r="D52" s="7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E52" s="7" t="n">
         <v>1</v>
@@ -2411,7 +2431,7 @@
     </row>
     <row r="53" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="6" t="n">
-        <v>44464</v>
+        <v>44474</v>
       </c>
       <c r="B53" s="7" t="n">
         <v>1</v>
@@ -2426,7 +2446,7 @@
         <v>1</v>
       </c>
       <c r="F53" s="7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G53" s="7" t="n">
         <v>1</v>
@@ -2446,13 +2466,11 @@
       <c r="L53" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="M53" s="7" t="s">
-        <v>13</v>
-      </c>
+      <c r="M53" s="7"/>
     </row>
     <row r="54" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="6" t="n">
-        <v>44463</v>
+        <v>44473</v>
       </c>
       <c r="B54" s="7" t="n">
         <v>1</v>
@@ -2467,7 +2485,7 @@
         <v>1</v>
       </c>
       <c r="F54" s="7" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G54" s="7" t="n">
         <v>1</v>
@@ -2487,13 +2505,11 @@
       <c r="L54" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="M54" s="7" t="s">
-        <v>13</v>
-      </c>
+      <c r="M54" s="7"/>
     </row>
     <row r="55" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="6" t="n">
-        <v>44462</v>
+        <v>44472</v>
       </c>
       <c r="B55" s="7" t="n">
         <v>1</v>
@@ -2528,16 +2544,14 @@
       <c r="L55" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="M55" s="7" t="s">
-        <v>13</v>
-      </c>
+      <c r="M55" s="7"/>
     </row>
     <row r="56" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="6" t="n">
-        <v>44461</v>
+        <v>44471</v>
       </c>
       <c r="B56" s="7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C56" s="7" t="n">
         <v>1</v>
@@ -2569,13 +2583,11 @@
       <c r="L56" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="M56" s="7" t="s">
-        <v>13</v>
-      </c>
+      <c r="M56" s="7"/>
     </row>
     <row r="57" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="6" t="n">
-        <v>44460</v>
+        <v>44470</v>
       </c>
       <c r="B57" s="7" t="n">
         <v>1</v>
@@ -2610,13 +2622,11 @@
       <c r="L57" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="M57" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="M57" s="7"/>
     </row>
     <row r="58" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="6" t="n">
-        <v>44459</v>
+        <v>44469</v>
       </c>
       <c r="B58" s="7" t="n">
         <v>1</v>
@@ -2631,7 +2641,7 @@
         <v>1</v>
       </c>
       <c r="F58" s="7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G58" s="7" t="n">
         <v>1</v>
@@ -2651,13 +2661,11 @@
       <c r="L58" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="M58" s="7" t="s">
-        <v>13</v>
-      </c>
+      <c r="M58" s="7"/>
     </row>
     <row r="59" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="6" t="n">
-        <v>44458</v>
+        <v>44468</v>
       </c>
       <c r="B59" s="7" t="n">
         <v>1</v>
@@ -2672,7 +2680,7 @@
         <v>1</v>
       </c>
       <c r="F59" s="7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G59" s="7" t="n">
         <v>1</v>
@@ -2692,13 +2700,11 @@
       <c r="L59" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="M59" s="7" t="s">
-        <v>13</v>
-      </c>
+      <c r="M59" s="7"/>
     </row>
     <row r="60" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="6" t="n">
-        <v>44457</v>
+        <v>44467</v>
       </c>
       <c r="B60" s="7" t="n">
         <v>1</v>
@@ -2713,7 +2719,7 @@
         <v>1</v>
       </c>
       <c r="F60" s="7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G60" s="7" t="n">
         <v>1</v>
@@ -2733,13 +2739,11 @@
       <c r="L60" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="M60" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="M60" s="7"/>
     </row>
     <row r="61" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="6" t="n">
-        <v>44456</v>
+        <v>44466</v>
       </c>
       <c r="B61" s="7" t="n">
         <v>1</v>
@@ -2754,7 +2758,7 @@
         <v>1</v>
       </c>
       <c r="F61" s="7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G61" s="7" t="n">
         <v>1</v>
@@ -2774,927 +2778,872 @@
       <c r="L61" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="M61" s="7" t="s">
-        <v>15</v>
-      </c>
+      <c r="M61" s="7"/>
     </row>
     <row r="62" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="6" t="n">
+        <v>44465</v>
+      </c>
+      <c r="B62" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C62" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D62" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E62" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F62" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G62" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H62" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I62" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J62" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K62" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L62" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M62" s="7"/>
+    </row>
+    <row r="63" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="6" t="n">
+        <v>44464</v>
+      </c>
+      <c r="B63" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C63" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D63" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E63" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F63" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G63" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H63" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I63" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J63" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K63" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L63" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M63" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="6" t="n">
+        <v>44463</v>
+      </c>
+      <c r="B64" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C64" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D64" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E64" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F64" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="G64" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H64" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I64" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J64" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K64" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L64" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M64" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="6" t="n">
+        <v>44462</v>
+      </c>
+      <c r="B65" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C65" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D65" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E65" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F65" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="G65" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H65" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I65" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J65" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K65" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L65" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M65" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="6" t="n">
+        <v>44461</v>
+      </c>
+      <c r="B66" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C66" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D66" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E66" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F66" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="G66" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H66" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I66" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J66" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K66" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L66" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M66" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="6" t="n">
+        <v>44460</v>
+      </c>
+      <c r="B67" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C67" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D67" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E67" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F67" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G67" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H67" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I67" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J67" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K67" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L67" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M67" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="6" t="n">
+        <v>44459</v>
+      </c>
+      <c r="B68" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C68" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D68" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E68" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F68" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G68" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H68" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I68" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J68" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K68" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L68" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M68" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A69" s="6" t="n">
+        <v>44458</v>
+      </c>
+      <c r="B69" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C69" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D69" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E69" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F69" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="G69" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H69" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I69" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J69" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K69" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L69" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M69" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="6" t="n">
+        <v>44457</v>
+      </c>
+      <c r="B70" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C70" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D70" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E70" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F70" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="G70" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H70" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I70" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J70" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K70" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L70" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M70" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="6" t="n">
+        <v>44456</v>
+      </c>
+      <c r="B71" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C71" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D71" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E71" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F71" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G71" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H71" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I71" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J71" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K71" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L71" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M71" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="6" t="n">
         <v>44455</v>
       </c>
-      <c r="B62" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C62" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D62" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E62" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F62" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G62" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H62" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="I62" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J62" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K62" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="L62" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M62" s="7" t="s">
+      <c r="B72" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C72" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D72" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E72" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F72" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G72" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H72" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I72" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J72" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K72" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L72" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M72" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="8" t="n">
+    <row r="73" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="8" t="n">
         <v>44454</v>
       </c>
-      <c r="B63" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C63" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D63" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E63" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F63" s="9" t="n">
+      <c r="B73" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C73" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D73" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E73" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F73" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="G63" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H63" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I63" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="J63" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="K63" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="L63" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="M63" s="9" t="s">
+      <c r="G73" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H73" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="I73" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J73" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="K73" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="L73" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="M73" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="8" t="n">
+    <row r="74" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="8" t="n">
         <v>44453</v>
       </c>
-      <c r="B64" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C64" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D64" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="E64" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F64" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="G64" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H64" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I64" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="J64" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="K64" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="L64" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="M64" s="9" t="s">
+      <c r="B74" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C74" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D74" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E74" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F74" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="G74" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H74" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="I74" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J74" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="K74" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="L74" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="M74" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="8" t="n">
+    <row r="75" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="8" t="n">
         <v>44452</v>
       </c>
-      <c r="B65" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C65" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D65" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E65" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F65" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G65" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H65" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I65" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="J65" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="K65" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="L65" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="M65" s="9" t="s">
+      <c r="B75" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C75" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D75" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E75" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F75" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G75" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H75" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="I75" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J75" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="K75" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="L75" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="M75" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="8" t="n">
+    <row r="76" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A76" s="8" t="n">
         <v>44451</v>
       </c>
-      <c r="B66" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C66" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D66" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E66" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F66" s="9" t="n">
+      <c r="B76" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C76" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D76" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E76" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F76" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="G66" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H66" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I66" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="J66" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="K66" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="L66" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="M66" s="9" t="s">
+      <c r="G76" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H76" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="I76" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J76" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="K76" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="L76" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="M76" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="8" t="n">
+    <row r="77" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A77" s="8" t="n">
         <v>44450</v>
       </c>
-      <c r="B67" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C67" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D67" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E67" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F67" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="G67" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H67" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I67" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="J67" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="K67" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="L67" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="M67" s="9" t="s">
+      <c r="B77" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C77" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D77" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E77" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F77" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="G77" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H77" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="I77" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J77" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="K77" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="L77" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="M77" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="8" t="n">
+    <row r="78" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A78" s="8" t="n">
         <v>44449</v>
       </c>
-      <c r="B68" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C68" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D68" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E68" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F68" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G68" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H68" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I68" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="J68" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="K68" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="L68" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="M68" s="9" t="s">
+      <c r="B78" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C78" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D78" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E78" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F78" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G78" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H78" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="I78" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J78" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="K78" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="L78" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="M78" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="2" t="n">
+    <row r="79" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A79" s="2" t="n">
         <v>44448</v>
       </c>
-      <c r="B69" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C69" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D69" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E69" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F69" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G69" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H69" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="I69" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J69" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K69" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="L69" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M69" s="9" t="s">
+      <c r="B79" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C79" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D79" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E79" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F79" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G79" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H79" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I79" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J79" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K79" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L79" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M79" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="2" t="n">
+    <row r="80" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A80" s="2" t="n">
         <v>44447</v>
       </c>
-      <c r="B70" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C70" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D70" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="E70" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F70" s="7" t="n">
+      <c r="B80" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C80" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D80" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E80" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F80" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="G70" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H70" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="I70" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J70" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K70" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="L70" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M70" s="7" t="s">
+      <c r="G80" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H80" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I80" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J80" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K80" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L80" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M80" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="2" t="n">
+    <row r="81" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A81" s="2" t="n">
         <v>44446</v>
       </c>
-      <c r="B71" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C71" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D71" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E71" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F71" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="G71" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H71" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="I71" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J71" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K71" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="L71" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M71" s="7" t="s">
+      <c r="B81" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C81" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D81" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E81" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F81" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="G81" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H81" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I81" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J81" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K81" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L81" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M81" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="2" t="n">
+    <row r="82" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A82" s="2" t="n">
         <v>44445</v>
       </c>
-      <c r="B72" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C72" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D72" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E72" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F72" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G72" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H72" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="I72" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J72" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K72" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="L72" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M72" s="7" t="s">
+      <c r="B82" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C82" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D82" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E82" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F82" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G82" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H82" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I82" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J82" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K82" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L82" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M82" s="7" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="2" t="n">
-        <v>44444</v>
-      </c>
-      <c r="B73" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C73" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D73" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E73" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F73" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="G73" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H73" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="I73" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J73" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K73" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="L73" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M73" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="2" t="n">
-        <v>44443</v>
-      </c>
-      <c r="B74" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C74" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D74" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E74" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F74" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G74" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H74" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="I74" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J74" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K74" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="L74" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M74" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="2" t="n">
-        <v>44442</v>
-      </c>
-      <c r="B75" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C75" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D75" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E75" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F75" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="G75" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H75" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="I75" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J75" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K75" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="L75" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M75" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="2" t="n">
-        <v>44441</v>
-      </c>
-      <c r="B76" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C76" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D76" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E76" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F76" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G76" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H76" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="I76" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J76" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K76" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="L76" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="M76" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="11" t="n">
-        <v>44440</v>
-      </c>
-      <c r="B77" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C77" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D77" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E77" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F77" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="G77" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H77" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="I77" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J77" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K77" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="L77" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="M77" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="11" t="n">
-        <v>44439</v>
-      </c>
-      <c r="B78" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C78" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D78" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E78" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F78" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="G78" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H78" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="I78" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J78" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K78" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="L78" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="M78" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="N78" s="12"/>
-      <c r="O78" s="7"/>
-      <c r="P78" s="7"/>
-      <c r="Q78" s="7"/>
-      <c r="R78" s="7"/>
-      <c r="S78" s="7"/>
-      <c r="T78" s="7"/>
-      <c r="U78" s="7"/>
-      <c r="V78" s="7"/>
-      <c r="W78" s="7"/>
-      <c r="X78" s="7"/>
-      <c r="Y78" s="7"/>
-      <c r="Z78" s="7"/>
-      <c r="AA78" s="12"/>
-      <c r="AB78" s="7"/>
-      <c r="AC78" s="7"/>
-      <c r="AD78" s="7"/>
-      <c r="AE78" s="7"/>
-      <c r="AF78" s="7"/>
-      <c r="AG78" s="7"/>
-      <c r="AH78" s="7"/>
-      <c r="AI78" s="7"/>
-      <c r="AJ78" s="7"/>
-      <c r="AK78" s="7"/>
-      <c r="AL78" s="7"/>
-      <c r="AM78" s="7"/>
-      <c r="AN78" s="12"/>
-      <c r="AO78" s="7"/>
-      <c r="AP78" s="7"/>
-      <c r="AQ78" s="7"/>
-      <c r="AR78" s="7"/>
-      <c r="AS78" s="7"/>
-      <c r="AT78" s="7"/>
-      <c r="AU78" s="7"/>
-      <c r="AV78" s="7"/>
-      <c r="AW78" s="7"/>
-      <c r="AX78" s="7"/>
-      <c r="AY78" s="7"/>
-      <c r="AZ78" s="7"/>
-      <c r="BA78" s="12"/>
-      <c r="BB78" s="7"/>
-      <c r="BC78" s="7"/>
-      <c r="BD78" s="7"/>
-      <c r="BE78" s="7"/>
-      <c r="BF78" s="7"/>
-      <c r="BG78" s="7"/>
-      <c r="BH78" s="7"/>
-      <c r="BI78" s="7"/>
-      <c r="BJ78" s="7"/>
-      <c r="BK78" s="7"/>
-      <c r="BL78" s="7"/>
-    </row>
-    <row r="79" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="11" t="n">
-        <v>44438</v>
-      </c>
-      <c r="B79" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C79" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D79" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E79" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F79" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G79" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H79" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="I79" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J79" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K79" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="L79" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="M79" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="11" t="n">
-        <v>44437</v>
-      </c>
-      <c r="B80" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C80" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="D80" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="E80" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F80" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="G80" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H80" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="I80" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J80" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K80" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="L80" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="M80" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="11" t="n">
-        <v>44436</v>
-      </c>
-      <c r="B81" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C81" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D81" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E81" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F81" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="G81" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H81" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="I81" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J81" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K81" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="L81" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="M81" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="11" t="n">
-        <v>44435</v>
-      </c>
-      <c r="B82" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C82" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D82" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E82" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F82" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G82" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H82" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="I82" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J82" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K82" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="L82" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="M82" s="10" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="n">
-        <v>44434</v>
-      </c>
-      <c r="B83" s="10" t="n">
+        <v>44444</v>
+      </c>
+      <c r="B83" s="7" t="n">
         <v>1</v>
       </c>
       <c r="C83" s="7" t="n">
@@ -3707,7 +3656,7 @@
         <v>1</v>
       </c>
       <c r="F83" s="7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G83" s="7" t="n">
         <v>1</v>
@@ -3727,13 +3676,13 @@
       <c r="L83" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="M83" s="10" t="s">
-        <v>13</v>
+      <c r="M83" s="7" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="n">
-        <v>44433</v>
+        <v>44443</v>
       </c>
       <c r="B84" s="7" t="n">
         <v>1</v>
@@ -3748,7 +3697,7 @@
         <v>1</v>
       </c>
       <c r="F84" s="7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G84" s="7" t="n">
         <v>1</v>
@@ -3774,7 +3723,7 @@
     </row>
     <row r="85" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="n">
-        <v>44432</v>
+        <v>44442</v>
       </c>
       <c r="B85" s="7" t="n">
         <v>1</v>
@@ -3789,7 +3738,7 @@
         <v>1</v>
       </c>
       <c r="F85" s="7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G85" s="7" t="n">
         <v>1</v>
@@ -3810,44 +3759,44 @@
         <v>1</v>
       </c>
       <c r="M85" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="n">
-        <v>44431</v>
+        <v>44441</v>
       </c>
       <c r="B86" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C86" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D86" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E86" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F86" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G86" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H86" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="I86" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J86" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K86" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="L86" s="7" t="n">
+      <c r="C86" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D86" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E86" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F86" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G86" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H86" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I86" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J86" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K86" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L86" s="10" t="n">
         <v>1</v>
       </c>
       <c r="M86" s="7" t="s">
@@ -3855,90 +3804,141 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="13" t="n">
-        <v>44430</v>
-      </c>
-      <c r="B87" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C87" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="D87" s="14" t="n">
-        <v>2</v>
-      </c>
-      <c r="E87" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="F87" s="14" t="n">
-        <v>4</v>
-      </c>
-      <c r="G87" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="H87" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="I87" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="J87" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="K87" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="L87" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="M87" s="14" t="s">
+      <c r="A87" s="11" t="n">
+        <v>44440</v>
+      </c>
+      <c r="B87" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C87" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D87" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E87" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F87" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="G87" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H87" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="I87" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J87" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K87" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L87" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M87" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="11" t="n">
+        <v>44439</v>
+      </c>
+      <c r="B88" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C88" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D88" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E88" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F88" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="G88" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H88" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I88" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J88" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K88" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L88" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M88" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="88" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="11" t="n">
-        <v>44429</v>
-      </c>
-      <c r="B88" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C88" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D88" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E88" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F88" s="10" t="n">
-        <v>4</v>
-      </c>
-      <c r="G88" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H88" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="I88" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J88" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K88" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="L88" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="M88" s="10" t="s">
-        <v>17</v>
-      </c>
+      <c r="N88" s="12"/>
+      <c r="O88" s="7"/>
+      <c r="P88" s="7"/>
+      <c r="Q88" s="7"/>
+      <c r="R88" s="7"/>
+      <c r="S88" s="7"/>
+      <c r="T88" s="7"/>
+      <c r="U88" s="7"/>
+      <c r="V88" s="7"/>
+      <c r="W88" s="7"/>
+      <c r="X88" s="7"/>
+      <c r="Y88" s="7"/>
+      <c r="Z88" s="7"/>
+      <c r="AA88" s="12"/>
+      <c r="AB88" s="7"/>
+      <c r="AC88" s="7"/>
+      <c r="AD88" s="7"/>
+      <c r="AE88" s="7"/>
+      <c r="AF88" s="7"/>
+      <c r="AG88" s="7"/>
+      <c r="AH88" s="7"/>
+      <c r="AI88" s="7"/>
+      <c r="AJ88" s="7"/>
+      <c r="AK88" s="7"/>
+      <c r="AL88" s="7"/>
+      <c r="AM88" s="7"/>
+      <c r="AN88" s="12"/>
+      <c r="AO88" s="7"/>
+      <c r="AP88" s="7"/>
+      <c r="AQ88" s="7"/>
+      <c r="AR88" s="7"/>
+      <c r="AS88" s="7"/>
+      <c r="AT88" s="7"/>
+      <c r="AU88" s="7"/>
+      <c r="AV88" s="7"/>
+      <c r="AW88" s="7"/>
+      <c r="AX88" s="7"/>
+      <c r="AY88" s="7"/>
+      <c r="AZ88" s="7"/>
+      <c r="BA88" s="12"/>
+      <c r="BB88" s="7"/>
+      <c r="BC88" s="7"/>
+      <c r="BD88" s="7"/>
+      <c r="BE88" s="7"/>
+      <c r="BF88" s="7"/>
+      <c r="BG88" s="7"/>
+      <c r="BH88" s="7"/>
+      <c r="BI88" s="7"/>
+      <c r="BJ88" s="7"/>
+      <c r="BK88" s="7"/>
+      <c r="BL88" s="7"/>
     </row>
     <row r="89" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="11" t="n">
-        <v>44428</v>
+        <v>44438</v>
       </c>
       <c r="B89" s="10" t="n">
         <v>1</v>
@@ -3953,7 +3953,7 @@
         <v>1</v>
       </c>
       <c r="F89" s="10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G89" s="10" t="n">
         <v>1</v>
@@ -3974,27 +3974,27 @@
         <v>1</v>
       </c>
       <c r="M89" s="10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="11" t="n">
-        <v>44427</v>
+        <v>44437</v>
       </c>
       <c r="B90" s="10" t="n">
         <v>1</v>
       </c>
       <c r="C90" s="10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D90" s="10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E90" s="10" t="n">
         <v>1</v>
       </c>
       <c r="F90" s="10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G90" s="10" t="n">
         <v>1</v>
@@ -4015,12 +4015,12 @@
         <v>1</v>
       </c>
       <c r="M90" s="10" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="11" t="n">
-        <v>44426</v>
+        <v>44436</v>
       </c>
       <c r="B91" s="10" t="n">
         <v>1</v>
@@ -4029,13 +4029,13 @@
         <v>1</v>
       </c>
       <c r="D91" s="10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E91" s="10" t="n">
         <v>1</v>
       </c>
       <c r="F91" s="10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G91" s="10" t="n">
         <v>1</v>
@@ -4056,12 +4056,12 @@
         <v>1</v>
       </c>
       <c r="M91" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="11" t="n">
-        <v>44425</v>
+        <v>44435</v>
       </c>
       <c r="B92" s="10" t="n">
         <v>1</v>
@@ -4076,7 +4076,7 @@
         <v>1</v>
       </c>
       <c r="F92" s="10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G92" s="10" t="n">
         <v>1</v>
@@ -4097,44 +4097,44 @@
         <v>1</v>
       </c>
       <c r="M92" s="10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="11" t="n">
-        <v>44424</v>
+      <c r="A93" s="2" t="n">
+        <v>44434</v>
       </c>
       <c r="B93" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="C93" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D93" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E93" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F93" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G93" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H93" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="I93" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J93" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K93" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="L93" s="10" t="n">
+      <c r="C93" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D93" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E93" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F93" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="G93" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H93" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I93" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J93" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K93" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L93" s="7" t="n">
         <v>1</v>
       </c>
       <c r="M93" s="10" t="s">
@@ -4142,425 +4142,835 @@
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A94" s="11" t="n">
+      <c r="A94" s="2" t="n">
+        <v>44433</v>
+      </c>
+      <c r="B94" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C94" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D94" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E94" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F94" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="G94" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H94" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I94" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J94" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K94" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L94" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M94" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A95" s="2" t="n">
+        <v>44432</v>
+      </c>
+      <c r="B95" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C95" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D95" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E95" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F95" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G95" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H95" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I95" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J95" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K95" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L95" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M95" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A96" s="2" t="n">
+        <v>44431</v>
+      </c>
+      <c r="B96" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C96" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D96" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E96" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F96" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G96" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H96" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I96" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J96" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K96" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L96" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M96" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A97" s="13" t="n">
+        <v>44430</v>
+      </c>
+      <c r="B97" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C97" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D97" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="E97" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F97" s="14" t="n">
+        <v>4</v>
+      </c>
+      <c r="G97" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="H97" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="I97" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="J97" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="K97" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="L97" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="M97" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A98" s="11" t="n">
+        <v>44429</v>
+      </c>
+      <c r="B98" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C98" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D98" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E98" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F98" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="G98" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H98" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I98" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J98" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K98" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L98" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M98" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A99" s="11" t="n">
+        <v>44428</v>
+      </c>
+      <c r="B99" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C99" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D99" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E99" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F99" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="G99" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H99" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I99" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J99" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K99" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L99" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M99" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A100" s="11" t="n">
+        <v>44427</v>
+      </c>
+      <c r="B100" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C100" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D100" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E100" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F100" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="G100" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H100" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I100" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J100" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K100" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L100" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M100" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A101" s="11" t="n">
+        <v>44426</v>
+      </c>
+      <c r="B101" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C101" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D101" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E101" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F101" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G101" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H101" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I101" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J101" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K101" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L101" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M101" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A102" s="11" t="n">
+        <v>44425</v>
+      </c>
+      <c r="B102" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C102" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D102" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E102" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F102" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="G102" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H102" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I102" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J102" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K102" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L102" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M102" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A103" s="11" t="n">
+        <v>44424</v>
+      </c>
+      <c r="B103" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C103" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D103" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E103" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F103" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G103" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H103" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I103" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J103" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K103" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L103" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M103" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A104" s="11" t="n">
         <v>44423</v>
       </c>
-      <c r="B94" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C94" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D94" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E94" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F94" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G94" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H94" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="I94" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J94" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K94" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="L94" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="M94" s="10" t="s">
+      <c r="B104" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C104" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D104" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E104" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F104" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G104" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H104" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I104" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J104" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K104" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L104" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M104" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="11" t="n">
+    <row r="105" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A105" s="11" t="n">
         <v>44422</v>
       </c>
-      <c r="B95" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C95" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D95" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E95" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F95" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="G95" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H95" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="I95" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J95" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K95" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="L95" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="M95" s="10" t="s">
+      <c r="B105" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C105" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D105" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E105" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F105" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="G105" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H105" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I105" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J105" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K105" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L105" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M105" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A96" s="11" t="n">
+    <row r="106" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A106" s="11" t="n">
         <v>44421</v>
       </c>
-      <c r="B96" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C96" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="D96" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="E96" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F96" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G96" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H96" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="I96" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J96" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K96" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="L96" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="M96" s="10" t="s">
+      <c r="B106" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C106" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D106" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E106" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F106" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G106" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H106" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="I106" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J106" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K106" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L106" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M106" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A97" s="11" t="n">
+    <row r="107" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A107" s="11" t="n">
         <v>44420</v>
       </c>
-      <c r="B97" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C97" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D97" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E97" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F97" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="G97" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H97" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="I97" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J97" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K97" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="L97" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="M97" s="10" t="s">
+      <c r="B107" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C107" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D107" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E107" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F107" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G107" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H107" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I107" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J107" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K107" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L107" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M107" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A98" s="2" t="n">
+    <row r="108" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A108" s="2" t="n">
         <v>44419</v>
       </c>
-      <c r="B98" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C98" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D98" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="E98" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F98" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="G98" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H98" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="I98" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J98" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K98" s="7"/>
-      <c r="L98" s="7"/>
-      <c r="M98" s="7" t="s">
+      <c r="B108" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C108" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D108" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E108" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F108" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="G108" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H108" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I108" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J108" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K108" s="7"/>
+      <c r="L108" s="7"/>
+      <c r="M108" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A99" s="2" t="n">
+    <row r="109" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A109" s="2" t="n">
         <v>44418</v>
       </c>
-      <c r="B99" s="7" t="n">
+      <c r="B109" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="C99" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D99" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E99" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F99" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G99" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="H99" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="I99" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J99" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K99" s="7"/>
-      <c r="L99" s="7"/>
-      <c r="M99" s="7" t="s">
+      <c r="C109" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D109" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E109" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F109" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G109" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="H109" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I109" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J109" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K109" s="7"/>
+      <c r="L109" s="7"/>
+      <c r="M109" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A100" s="2" t="n">
+    <row r="110" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A110" s="2" t="n">
         <v>44417</v>
       </c>
-      <c r="B100" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C100" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D100" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E100" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F100" s="7" t="n">
+      <c r="B110" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C110" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D110" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E110" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F110" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="G100" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H100" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="I100" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J100" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K100" s="7"/>
-      <c r="L100" s="7"/>
-      <c r="M100" s="7" t="s">
+      <c r="G110" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H110" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I110" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J110" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K110" s="7"/>
+      <c r="L110" s="7"/>
+      <c r="M110" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A101" s="2" t="n">
+    <row r="111" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A111" s="2" t="n">
         <v>44416</v>
       </c>
-      <c r="B101" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C101" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D101" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E101" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F101" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="G101" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H101" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="I101" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J101" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K101" s="7"/>
-      <c r="L101" s="7"/>
-      <c r="M101" s="7" t="s">
+      <c r="B111" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C111" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D111" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E111" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F111" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="G111" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H111" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I111" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J111" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K111" s="7"/>
+      <c r="L111" s="7"/>
+      <c r="M111" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A102" s="2" t="n">
+    <row r="112" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A112" s="2" t="n">
         <v>44415</v>
       </c>
-      <c r="B102" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C102" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D102" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E102" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F102" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G102" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H102" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="I102" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J102" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K102" s="7"/>
-      <c r="L102" s="7"/>
-      <c r="M102" s="7" t="s">
+      <c r="B112" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C112" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D112" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E112" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F112" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G112" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H112" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I112" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J112" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K112" s="7"/>
+      <c r="L112" s="7"/>
+      <c r="M112" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A103" s="2" t="n">
+    <row r="113" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A113" s="2" t="n">
         <v>44414</v>
       </c>
-      <c r="B103" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C103" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D103" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E103" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F103" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="G103" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H103" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="I103" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J103" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K103" s="7"/>
-      <c r="L103" s="7"/>
-      <c r="M103" s="7" t="s">
+      <c r="B113" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C113" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D113" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E113" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F113" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="G113" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H113" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I113" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J113" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K113" s="7"/>
+      <c r="L113" s="7"/>
+      <c r="M113" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A104" s="2" t="n">
+    <row r="114" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A114" s="2" t="n">
         <v>44413</v>
       </c>
-      <c r="B104" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C104" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D104" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E104" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F104" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G104" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H104" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="I104" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J104" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K104" s="7"/>
-      <c r="L104" s="7"/>
-      <c r="M104" s="7" t="s">
+      <c r="B114" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C114" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D114" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E114" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F114" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G114" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H114" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I114" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J114" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K114" s="7"/>
+      <c r="L114" s="7"/>
+      <c r="M114" s="7" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>